<commit_message>
new changes and email
</commit_message>
<xml_diff>
--- a/uploads/bulk_skeletons/product.xlsx
+++ b/uploads/bulk_skeletons/product.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>title</t>
   </si>
@@ -25,12 +25,6 @@
     <t>category</t>
   </si>
   <si>
-    <t>sub_category</t>
-  </si>
-  <si>
-    <t>brand</t>
-  </si>
-  <si>
     <t>purchase_price</t>
   </si>
   <si>
@@ -40,32 +34,29 @@
     <t>discount</t>
   </si>
   <si>
-    <t>tax</t>
-  </si>
-  <si>
-    <t>shipping_cost</t>
-  </si>
-  <si>
     <t>add_stock</t>
   </si>
   <si>
     <t>images</t>
   </si>
   <si>
-    <t>tag</t>
-  </si>
-  <si>
-    <t>unit</t>
-  </si>
-  <si>
     <t>published</t>
+  </si>
+  <si>
+    <t>title_ar</t>
+  </si>
+  <si>
+    <t>description_ar</t>
+  </si>
+  <si>
+    <t>sku_number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,7 +147,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -188,10 +179,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -223,7 +213,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -399,71 +388,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="8" max="8" width="4.5546875" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
     <col min="9" max="9" width="9" customWidth="1"/>
     <col min="10" max="10" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>